<commit_message>
tweaked thresholds and added functionality to write to MLS xl file
</commit_message>
<xml_diff>
--- a/TestFiles/MLSData.xlsx
+++ b/TestFiles/MLSData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\Source\Repos\BuschEric97\HatcoFilesClosedDeterminer\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D1AC65-F190-4F9C-A90D-F9DB5D4E730B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA2186F-A2FC-4C6F-9573-F6DB17AAA106}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -579,18 +579,18 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="J11" sqref="J2:J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="16.109375" customWidth="1"/>
-    <col min="5" max="5" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" customWidth="1"/>
-    <col min="7" max="10" width="16.109375" customWidth="1"/>
+    <col min="1" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="10" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -622,7 +622,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -651,7 +651,7 @@
         <v>61900</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -680,7 +680,7 @@
         <v>135000</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -709,7 +709,7 @@
         <v>142500</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -738,7 +738,7 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -767,7 +767,7 @@
         <v>227000</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -796,7 +796,7 @@
         <v>110000</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -825,7 +825,7 @@
         <v>293000</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -854,7 +854,7 @@
         <v>75000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -883,7 +883,7 @@
         <v>325000</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
Added open file buttons, they currently hang when clicked
</commit_message>
<xml_diff>
--- a/TestFiles/MLSData.xlsx
+++ b/TestFiles/MLSData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\Source\Repos\BuschEric97\HatcoFilesClosedDeterminer\TestFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\source\repos\WindowsFormsApp1\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2410701C-929F-4988-867B-C7191FD5711E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E11C524-E92B-49D7-ADCC-A5F5432F1717}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30900" yWindow="2895" windowWidth="21600" windowHeight="11385" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -578,19 +578,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{807ACA53-ECA1-4FB2-BF4A-6452718DE0C4}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J2:J11"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="10" width="16.140625" customWidth="1"/>
+    <col min="1" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
+    <col min="7" max="10" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -622,7 +622,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -651,7 +651,7 @@
         <v>61900</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -680,7 +680,7 @@
         <v>135000</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -709,7 +709,7 @@
         <v>142500</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -738,7 +738,7 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -767,7 +767,7 @@
         <v>227000</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -796,7 +796,7 @@
         <v>110000</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -825,7 +825,7 @@
         <v>293000</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -854,7 +854,7 @@
         <v>75000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -883,7 +883,7 @@
         <v>325000</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
Added console messages for saving and closing workbooks
</commit_message>
<xml_diff>
--- a/TestFiles/MLSData.xlsx
+++ b/TestFiles/MLSData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\source\repos\WindowsFormsApp1\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E11C524-E92B-49D7-ADCC-A5F5432F1717}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D58020-6185-489D-AB29-04B4B30BAE9E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -579,7 +579,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added message box to show completion
</commit_message>
<xml_diff>
--- a/TestFiles/MLSData.xlsx
+++ b/TestFiles/MLSData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\source\repos\WindowsFormsApp1\TestFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\source\repos\BuschEric97\HatcoFilesClosedDeterminer\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D58020-6185-489D-AB29-04B4B30BAE9E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E772D0-D3E3-4CA5-AAEE-AB02AF6243E4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
   <si>
     <t>Selling Agent</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>425 E Johnson Street</t>
+  </si>
+  <si>
+    <t>did not close</t>
   </si>
 </sst>
 </file>
@@ -582,15 +585,15 @@
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="16.109375" customWidth="1"/>
-    <col min="5" max="5" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" customWidth="1"/>
-    <col min="7" max="10" width="16.109375" customWidth="1"/>
+    <col min="1" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="10" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -622,7 +625,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -650,8 +653,11 @@
       <c r="I2" s="2">
         <v>61900</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J2">
+        <v>20191011</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -679,8 +685,11 @@
       <c r="I3" s="2">
         <v>135000</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J3">
+        <v>20191062</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -708,8 +717,11 @@
       <c r="I4" s="2">
         <v>142500</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -737,8 +749,11 @@
       <c r="I5" s="2">
         <v>250000</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -766,8 +781,11 @@
       <c r="I6" s="2">
         <v>227000</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -795,8 +813,11 @@
       <c r="I7" s="2">
         <v>110000</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -824,8 +845,11 @@
       <c r="I8" s="2">
         <v>293000</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -853,8 +877,11 @@
       <c r="I9" s="2">
         <v>75000</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -882,8 +909,11 @@
       <c r="I10" s="2">
         <v>325000</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J10">
+        <v>20182625</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -910,6 +940,9 @@
       </c>
       <c r="I11" s="2">
         <v>130000</v>
+      </c>
+      <c r="J11" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit so I can pull
</commit_message>
<xml_diff>
--- a/TestFiles/MLSData.xlsx
+++ b/TestFiles/MLSData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\source\repos\WindowsFormsApp1\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D58020-6185-489D-AB29-04B4B30BAE9E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A79831B-5F8E-41A4-A6AF-867A0ED7683A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -579,7 +579,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="J11" sqref="J2:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fixed issue with reading AIM file and added new test file
</commit_message>
<xml_diff>
--- a/TestFiles/MLSData.xlsx
+++ b/TestFiles/MLSData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\source\repos\BuschEric97\HatcoFilesClosedDeterminer\TestFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\source\repos\WindowsFormsApp1\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E772D0-D3E3-4CA5-AAEE-AB02AF6243E4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6BF441-88E0-496E-8BA6-E95BE2F348CB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="63">
   <si>
     <t>Selling Agent</t>
   </si>
@@ -220,9 +220,6 @@
   </si>
   <si>
     <t>425 E Johnson Street</t>
-  </si>
-  <si>
-    <t>did not close</t>
   </si>
 </sst>
 </file>
@@ -582,18 +579,18 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="J11" sqref="J2:J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="10" width="16.140625" customWidth="1"/>
+    <col min="1" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
+    <col min="7" max="10" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -625,7 +622,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -653,11 +650,8 @@
       <c r="I2" s="2">
         <v>61900</v>
       </c>
-      <c r="J2">
-        <v>20191011</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -685,11 +679,8 @@
       <c r="I3" s="2">
         <v>135000</v>
       </c>
-      <c r="J3">
-        <v>20191062</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -717,11 +708,8 @@
       <c r="I4" s="2">
         <v>142500</v>
       </c>
-      <c r="J4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -749,11 +737,8 @@
       <c r="I5" s="2">
         <v>250000</v>
       </c>
-      <c r="J5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -781,11 +766,8 @@
       <c r="I6" s="2">
         <v>227000</v>
       </c>
-      <c r="J6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -813,11 +795,8 @@
       <c r="I7" s="2">
         <v>110000</v>
       </c>
-      <c r="J7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -845,11 +824,8 @@
       <c r="I8" s="2">
         <v>293000</v>
       </c>
-      <c r="J8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -877,11 +853,8 @@
       <c r="I9" s="2">
         <v>75000</v>
       </c>
-      <c r="J9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -909,11 +882,8 @@
       <c r="I10" s="2">
         <v>325000</v>
       </c>
-      <c r="J10">
-        <v>20182625</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -940,9 +910,6 @@
       </c>
       <c r="I11" s="2">
         <v>130000</v>
-      </c>
-      <c r="J11" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added progress bar to program
</commit_message>
<xml_diff>
--- a/TestFiles/MLSData.xlsx
+++ b/TestFiles/MLSData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\source\repos\WindowsFormsApp1\TestFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\Source\Repos\BuschEric97\HatcoFilesClosedDeterminer\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6BF441-88E0-496E-8BA6-E95BE2F348CB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0084B537-3AC9-40A8-AB30-60639254012C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -579,18 +579,18 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J2:J11"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="16.109375" customWidth="1"/>
-    <col min="5" max="5" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" customWidth="1"/>
-    <col min="7" max="10" width="16.109375" customWidth="1"/>
+    <col min="1" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="10" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -622,7 +622,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -651,7 +651,7 @@
         <v>61900</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -680,7 +680,7 @@
         <v>135000</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -709,7 +709,7 @@
         <v>142500</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -738,7 +738,7 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -767,7 +767,7 @@
         <v>227000</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -796,7 +796,7 @@
         <v>110000</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -825,7 +825,7 @@
         <v>293000</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -854,7 +854,7 @@
         <v>75000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -883,7 +883,7 @@
         <v>325000</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
Reformatted code and fixed bug where files are held hostage on program crash
</commit_message>
<xml_diff>
--- a/TestFiles/MLSData.xlsx
+++ b/TestFiles/MLSData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\Source\Repos\BuschEric97\HatcoFilesClosedDeterminer\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0084B537-3AC9-40A8-AB30-60639254012C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A48EFE4-18DA-4395-811B-F01A5A482BF4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
   </bookViews>
@@ -579,7 +579,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="J11" sqref="J2:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Reformatted code to use dictionaries for several variables
</commit_message>
<xml_diff>
--- a/TestFiles/MLSData.xlsx
+++ b/TestFiles/MLSData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\Source\Repos\BuschEric97\HatcoFilesClosedDeterminer\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A48EFE4-18DA-4395-811B-F01A5A482BF4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C19CB2-44DB-4132-9A37-B148E384DD29}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
   </bookViews>
@@ -579,7 +579,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J2:J11"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
modified progress bar implementation
</commit_message>
<xml_diff>
--- a/TestFiles/MLSData.xlsx
+++ b/TestFiles/MLSData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\Source\Repos\BuschEric97\HatcoFilesClosedDeterminer\TestFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\source\repos\BuschEric97\HatcoFilesClosedDeterminer\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C19CB2-44DB-4132-9A37-B148E384DD29}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA90AA5-D0ED-4A55-AB8D-15FA236FA4B9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
   <si>
     <t>Selling Agent</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>425 E Johnson Street</t>
+  </si>
+  <si>
+    <t>did not close</t>
   </si>
 </sst>
 </file>
@@ -650,6 +653,9 @@
       <c r="I2" s="2">
         <v>61900</v>
       </c>
+      <c r="J2">
+        <v>20191011</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -679,6 +685,9 @@
       <c r="I3" s="2">
         <v>135000</v>
       </c>
+      <c r="J3">
+        <v>20191062</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -708,6 +717,9 @@
       <c r="I4" s="2">
         <v>142500</v>
       </c>
+      <c r="J4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -737,6 +749,9 @@
       <c r="I5" s="2">
         <v>250000</v>
       </c>
+      <c r="J5" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -766,6 +781,9 @@
       <c r="I6" s="2">
         <v>227000</v>
       </c>
+      <c r="J6" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -795,6 +813,9 @@
       <c r="I7" s="2">
         <v>110000</v>
       </c>
+      <c r="J7" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -824,6 +845,9 @@
       <c r="I8" s="2">
         <v>293000</v>
       </c>
+      <c r="J8" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -853,6 +877,9 @@
       <c r="I9" s="2">
         <v>75000</v>
       </c>
+      <c r="J9" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -882,6 +909,9 @@
       <c r="I10" s="2">
         <v>325000</v>
       </c>
+      <c r="J10">
+        <v>20182625</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -910,6 +940,9 @@
       </c>
       <c r="I11" s="2">
         <v>130000</v>
+      </c>
+      <c r="J11" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started multithreading. Problems with mutex lock
</commit_message>
<xml_diff>
--- a/TestFiles/MLSData.xlsx
+++ b/TestFiles/MLSData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\source\repos\BuschEric97\HatcoFilesClosedDeterminer\TestFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\Source\Repos\BuschEric97\HatcoFilesClosedDeterminer\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA90AA5-D0ED-4A55-AB8D-15FA236FA4B9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66F9075-4FE2-46C0-9A75-FDBD55DD88BA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="63">
   <si>
     <t>Selling Agent</t>
   </si>
@@ -220,9 +220,6 @@
   </si>
   <si>
     <t>425 E Johnson Street</t>
-  </si>
-  <si>
-    <t>did not close</t>
   </si>
 </sst>
 </file>
@@ -582,7 +579,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,9 +650,6 @@
       <c r="I2" s="2">
         <v>61900</v>
       </c>
-      <c r="J2">
-        <v>20191011</v>
-      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -685,9 +679,6 @@
       <c r="I3" s="2">
         <v>135000</v>
       </c>
-      <c r="J3">
-        <v>20191062</v>
-      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -717,9 +708,6 @@
       <c r="I4" s="2">
         <v>142500</v>
       </c>
-      <c r="J4" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -749,9 +737,6 @@
       <c r="I5" s="2">
         <v>250000</v>
       </c>
-      <c r="J5" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -781,9 +766,6 @@
       <c r="I6" s="2">
         <v>227000</v>
       </c>
-      <c r="J6" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -813,9 +795,6 @@
       <c r="I7" s="2">
         <v>110000</v>
       </c>
-      <c r="J7" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -845,9 +824,6 @@
       <c r="I8" s="2">
         <v>293000</v>
       </c>
-      <c r="J8" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -877,9 +853,6 @@
       <c r="I9" s="2">
         <v>75000</v>
       </c>
-      <c r="J9" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -909,9 +882,6 @@
       <c r="I10" s="2">
         <v>325000</v>
       </c>
-      <c r="J10">
-        <v>20182625</v>
-      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -940,9 +910,6 @@
       </c>
       <c r="I11" s="2">
         <v>130000</v>
-      </c>
-      <c r="J11" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continued multithreading. Still doesn't work as intended
</commit_message>
<xml_diff>
--- a/TestFiles/MLSData.xlsx
+++ b/TestFiles/MLSData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\Source\Repos\BuschEric97\HatcoFilesClosedDeterminer\TestFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\source\repos\BuschEric97\HatcoFilesClosedDeterminer\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66F9075-4FE2-46C0-9A75-FDBD55DD88BA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DE6C36-87A4-43E4-B541-A1F1FD55BE30}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="64">
   <si>
     <t>Selling Agent</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>425 E Johnson Street</t>
+  </si>
+  <si>
+    <t>did not close</t>
   </si>
 </sst>
 </file>
@@ -579,7 +582,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="J11" sqref="J2:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,6 +653,9 @@
       <c r="I2" s="2">
         <v>61900</v>
       </c>
+      <c r="J2">
+        <v>20191011</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -679,6 +685,9 @@
       <c r="I3" s="2">
         <v>135000</v>
       </c>
+      <c r="J3">
+        <v>20191062</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -708,6 +717,9 @@
       <c r="I4" s="2">
         <v>142500</v>
       </c>
+      <c r="J4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -737,6 +749,9 @@
       <c r="I5" s="2">
         <v>250000</v>
       </c>
+      <c r="J5" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -766,6 +781,9 @@
       <c r="I6" s="2">
         <v>227000</v>
       </c>
+      <c r="J6" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -795,6 +813,9 @@
       <c r="I7" s="2">
         <v>110000</v>
       </c>
+      <c r="J7" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -824,6 +845,9 @@
       <c r="I8" s="2">
         <v>293000</v>
       </c>
+      <c r="J8">
+        <v>20190096</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -853,6 +877,9 @@
       <c r="I9" s="2">
         <v>75000</v>
       </c>
+      <c r="J9" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -882,6 +909,9 @@
       <c r="I10" s="2">
         <v>325000</v>
       </c>
+      <c r="J10">
+        <v>20182625</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -910,6 +940,9 @@
       </c>
       <c r="I11" s="2">
         <v>130000</v>
+      </c>
+      <c r="J11" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added some functionality, still need to tweak thresholds
</commit_message>
<xml_diff>
--- a/TestFiles/MLSData.xlsx
+++ b/TestFiles/MLSData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\source\repos\BuschEric97\HatcoFilesClosedDeterminer\TestFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\source\repos\WindowsFormsApp1\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA90AA5-D0ED-4A55-AB8D-15FA236FA4B9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F80E78C-097C-4308-904C-70ABA89C7AB9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -585,15 +585,15 @@
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="10" width="16.140625" customWidth="1"/>
+    <col min="1" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
+    <col min="7" max="10" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -625,7 +625,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -657,7 +657,7 @@
         <v>20191011</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -689,7 +689,7 @@
         <v>20191062</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -721,7 +721,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -753,7 +753,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -785,7 +785,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -817,7 +817,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -849,7 +849,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -881,7 +881,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -913,7 +913,7 @@
         <v>20182625</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
Added address parsing package
</commit_message>
<xml_diff>
--- a/TestFiles/MLSData.xlsx
+++ b/TestFiles/MLSData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\source\repos\WindowsFormsApp1\TestFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\Source\Repos\BuschEric97\HatcoFilesClosedDeterminer\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F80E78C-097C-4308-904C-70ABA89C7AB9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF91DD3-BCEE-4111-9A0F-8E68930A7E68}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="63">
   <si>
     <t>Selling Agent</t>
   </si>
@@ -220,9 +220,6 @@
   </si>
   <si>
     <t>425 E Johnson Street</t>
-  </si>
-  <si>
-    <t>did not close</t>
   </si>
 </sst>
 </file>
@@ -582,18 +579,18 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="16.109375" customWidth="1"/>
-    <col min="5" max="5" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" customWidth="1"/>
-    <col min="7" max="10" width="16.109375" customWidth="1"/>
+    <col min="1" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="10" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -625,7 +622,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -653,11 +650,8 @@
       <c r="I2" s="2">
         <v>61900</v>
       </c>
-      <c r="J2">
-        <v>20191011</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -685,11 +679,8 @@
       <c r="I3" s="2">
         <v>135000</v>
       </c>
-      <c r="J3">
-        <v>20191062</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -717,11 +708,8 @@
       <c r="I4" s="2">
         <v>142500</v>
       </c>
-      <c r="J4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -749,11 +737,8 @@
       <c r="I5" s="2">
         <v>250000</v>
       </c>
-      <c r="J5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -781,11 +766,8 @@
       <c r="I6" s="2">
         <v>227000</v>
       </c>
-      <c r="J6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -813,11 +795,8 @@
       <c r="I7" s="2">
         <v>110000</v>
       </c>
-      <c r="J7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -845,11 +824,8 @@
       <c r="I8" s="2">
         <v>293000</v>
       </c>
-      <c r="J8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -877,11 +853,8 @@
       <c r="I9" s="2">
         <v>75000</v>
       </c>
-      <c r="J9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -909,11 +882,8 @@
       <c r="I10" s="2">
         <v>325000</v>
       </c>
-      <c r="J10">
-        <v>20182625</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -940,9 +910,6 @@
       </c>
       <c r="I11" s="2">
         <v>130000</v>
-      </c>
-      <c r="J11" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated things to improve accuracy
</commit_message>
<xml_diff>
--- a/TestFiles/MLSData.xlsx
+++ b/TestFiles/MLSData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\Source\Repos\BuschEric97\HatcoFilesClosedDeterminer\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF91DD3-BCEE-4111-9A0F-8E68930A7E68}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A05641-14F9-412A-A1C0-21CD2BD633E6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B477FE81-BBEC-4E02-88DD-D51E7F5F506A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -579,7 +579,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="J11" sqref="J2:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>